<commit_message>
Q3 2025 SNA Update
</commit_message>
<xml_diff>
--- a/Data/National Accounts/PSA-Quarter-Q1-1981-to-latest.xlsx
+++ b/Data/National Accounts/PSA-Quarter-Q1-1981-to-latest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Shared drives\QNAP\NAP Dissemination\As of August 2025\Tables\Prelim Q2 2025\NAP 1981 and 1946 series\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Shared drives\QNAP\NAP Dissemination\As of November 2025\Tables\Prelim Q3 2025\NAP 1981 and 1946 series\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6351887-2B0F-459E-81E2-A1962ECFEBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961710AE-CBA2-4F65-B592-B134F242ED61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="721" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2456" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2468" uniqueCount="86">
   <si>
     <t>Source: Philippine Statistics Authority</t>
   </si>
@@ -229,13 +229,13 @@
     <t>3. Services</t>
   </si>
   <si>
-    <t>Q1 1981 to Q2 2025</t>
+    <t>Q1 1981 to Q3 2025</t>
   </si>
   <si>
-    <t>Q1 1982 to Q2 2025</t>
+    <t>Q1 1982 to Q3 2025</t>
   </si>
   <si>
-    <t>As of August 2025</t>
+    <t>As of November 2025</t>
   </si>
   <si>
     <t>1981 - 1982</t>
@@ -375,11 +375,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="#,##0;\-#,##0;\-;@"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="#,##0;\-#,##0;\-;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -445,9 +445,9 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -462,18 +462,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -486,7 +486,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma 2" xfId="1" xr:uid="{EBC8978A-E69D-4FF4-B0D2-6466C5361FC7}"/>
@@ -860,11 +860,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:FW304"/>
+  <dimension ref="A1:FX304"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="FE1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <pane xSplit="1" topLeftCell="FF1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="FX15" sqref="FX15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -993,41 +993,41 @@
     <col min="162" max="162" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="163" max="164" width="15.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="165" max="165" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="166" max="179" width="15" style="1" customWidth="1"/>
-    <col min="180" max="16384" width="9.28515625" style="1"/>
+    <col min="166" max="180" width="15" style="1" customWidth="1"/>
+    <col min="181" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="5">
         <v>1981</v>
@@ -1297,8 +1297,9 @@
         <v>2025</v>
       </c>
       <c r="FW9" s="5"/>
+      <c r="FX9" s="5"/>
     </row>
-    <row r="10" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1836,8 +1837,11 @@
       <c r="FW10" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="FX10" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="12" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -2373,10 +2377,13 @@
         <v>5151591.0908282408</v>
       </c>
       <c r="FW12" s="6">
-        <v>5028483.7627761383</v>
+        <v>5026487.6453204593</v>
+      </c>
+      <c r="FX12" s="6">
+        <v>5189616.6763309967</v>
       </c>
     </row>
-    <row r="13" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -2912,10 +2919,13 @@
         <v>976284.70268515893</v>
       </c>
       <c r="FW13" s="6">
-        <v>1176980.2565241435</v>
+        <v>1177074.1272160839</v>
+      </c>
+      <c r="FX13" s="6">
+        <v>1015913.3675783979</v>
       </c>
     </row>
-    <row r="14" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -3451,10 +3461,13 @@
         <v>1472266.2540826388</v>
       </c>
       <c r="FW14" s="6">
-        <v>1815653.2823573002</v>
+        <v>1827808.4661680828</v>
+      </c>
+      <c r="FX14" s="6">
+        <v>1471665.10236228</v>
       </c>
     </row>
-    <row r="15" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -3990,10 +4003,13 @@
         <v>1868965.9037470724</v>
       </c>
       <c r="FW15" s="6">
-        <v>1688589.8694190304</v>
+        <v>1692148.4795949869</v>
+      </c>
+      <c r="FX15" s="6">
+        <v>1889733.2701689133</v>
       </c>
     </row>
-    <row r="16" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -4529,10 +4545,13 @@
         <v>2848457.1551647144</v>
       </c>
       <c r="FW16" s="6">
-        <v>2697785.3154594307</v>
+        <v>2713878.5466870032</v>
+      </c>
+      <c r="FX16" s="6">
+        <v>2964470.3332322715</v>
       </c>
     </row>
-    <row r="17" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -5068,10 +5087,13 @@
         <v>-38563.940810134634</v>
       </c>
       <c r="FW17" s="6">
-        <v>-46829.443755216897</v>
+        <v>-44404.970106712542</v>
+      </c>
+      <c r="FX17" s="6">
+        <v>-44479.567014624365</v>
       </c>
     </row>
-    <row r="18" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:180" x14ac:dyDescent="0.2">
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -5250,8 +5272,9 @@
       <c r="FU18" s="6"/>
       <c r="FV18" s="6"/>
       <c r="FW18" s="6"/>
+      <c r="FX18" s="6"/>
     </row>
-    <row r="19" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>10</v>
       </c>
@@ -5787,14 +5810,17 @@
         <v>6582086.8553682622</v>
       </c>
       <c r="FW19" s="6">
-        <v>6965092.4118619654</v>
+        <v>6965235.2015058966</v>
+      </c>
+      <c r="FX19" s="6">
+        <v>6557978.5161936916</v>
       </c>
     </row>
-    <row r="20" spans="1:179" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:179" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:179" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:179" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:179" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:180" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -5974,43 +6000,44 @@
       <c r="FU24" s="8"/>
       <c r="FV24" s="8"/>
       <c r="FW24" s="8"/>
+      <c r="FX24" s="8"/>
     </row>
-    <row r="25" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="5">
         <v>1981</v>
@@ -6280,8 +6307,9 @@
         <v>2025</v>
       </c>
       <c r="FW36" s="5"/>
+      <c r="FX36" s="5"/>
     </row>
-    <row r="37" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>14</v>
       </c>
@@ -6819,8 +6847,11 @@
       <c r="FW37" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="FX37" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="39" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>1</v>
       </c>
@@ -7356,10 +7387,13 @@
         <v>4069803.2548084343</v>
       </c>
       <c r="FW39" s="6">
-        <v>3958652.3705736278</v>
+        <v>3953573.6827925313</v>
+      </c>
+      <c r="FX39" s="6">
+        <v>4033096.4016607953</v>
       </c>
     </row>
-    <row r="40" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>2</v>
       </c>
@@ -7895,10 +7929,13 @@
         <v>871001.67111655301</v>
       </c>
       <c r="FW40" s="6">
-        <v>1019861.6453696742</v>
+        <v>1019939.7254053591</v>
+      </c>
+      <c r="FX40" s="6">
+        <v>827191.36472739803</v>
       </c>
     </row>
-    <row r="41" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>3</v>
       </c>
@@ -8434,10 +8471,13 @@
         <v>1204467.4532642846</v>
       </c>
       <c r="FW41" s="6">
-        <v>1520196.5731796846</v>
+        <v>1528849.9073117932</v>
+      </c>
+      <c r="FX41" s="6">
+        <v>1186144.0174397747</v>
       </c>
     </row>
-    <row r="42" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
@@ -8973,10 +9013,13 @@
         <v>1590556.358413341</v>
       </c>
       <c r="FW42" s="6">
-        <v>1543537.7432285068</v>
+        <v>1548233.6101455386</v>
+      </c>
+      <c r="FX42" s="6">
+        <v>1664071.6682024854</v>
       </c>
     </row>
-    <row r="43" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>5</v>
       </c>
@@ -9512,10 +9555,13 @@
         <v>2236238.8480259255</v>
       </c>
       <c r="FW43" s="6">
-        <v>2176244.9081096733</v>
+        <v>2189147.1562115205</v>
+      </c>
+      <c r="FX43" s="6">
+        <v>2207932.9951640414</v>
       </c>
     </row>
-    <row r="44" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>6</v>
       </c>
@@ -10051,10 +10097,13 @@
         <v>-24512.185236306861</v>
       </c>
       <c r="FW44" s="6">
-        <v>-23603.23910403531</v>
+        <v>-18412.94380323682</v>
+      </c>
+      <c r="FX44" s="6">
+        <v>26264.142053938471</v>
       </c>
     </row>
-    <row r="45" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:180" x14ac:dyDescent="0.2">
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
@@ -10233,8 +10282,9 @@
       <c r="FU45" s="6"/>
       <c r="FV45" s="6"/>
       <c r="FW45" s="6"/>
+      <c r="FX45" s="6"/>
     </row>
-    <row r="46" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>10</v>
       </c>
@@ -10770,14 +10820,17 @@
         <v>5475077.7043403815</v>
       </c>
       <c r="FW46" s="6">
-        <v>5842400.1851377841</v>
+        <v>5843036.8256404642</v>
+      </c>
+      <c r="FX46" s="6">
+        <v>5528834.5989203509</v>
       </c>
     </row>
-    <row r="47" spans="1:179" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:179" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="1:179" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" spans="1:179" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" spans="1:179" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="1:180" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
@@ -10957,45 +11010,50 @@
       <c r="FU51" s="8"/>
       <c r="FV51" s="8"/>
       <c r="FW51" s="8"/>
+      <c r="FX51" s="8"/>
     </row>
-    <row r="52" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>40</v>
       </c>
+      <c r="FU60"/>
+      <c r="FV60"/>
+      <c r="FW60"/>
     </row>
-    <row r="61" spans="1:179" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="FR61"/>
+      <c r="FU61"/>
       <c r="FV61"/>
+      <c r="FW61"/>
     </row>
-    <row r="62" spans="1:179" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
@@ -11121,9 +11179,12 @@
       <c r="FH62" s="9"/>
       <c r="FL62" s="8"/>
       <c r="FP62" s="8"/>
+      <c r="FT62" s="8"/>
+      <c r="FU62"/>
       <c r="FV62"/>
+      <c r="FW62"/>
     </row>
-    <row r="63" spans="1:179" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="5" t="s">
         <v>42</v>
@@ -11387,9 +11448,12 @@
         <v>85</v>
       </c>
       <c r="FS63" s="5"/>
+      <c r="FT63" s="5"/>
+      <c r="FU63"/>
       <c r="FV63"/>
+      <c r="FW63"/>
     </row>
-    <row r="64" spans="1:179" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>14</v>
       </c>
@@ -11915,9 +11979,14 @@
       <c r="FS64" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="FT64" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="FU64"/>
       <c r="FV64"/>
+      <c r="FW64"/>
     </row>
-    <row r="65" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="B65" s="9"/>
       <c r="C65" s="10"/>
       <c r="D65" s="10"/>
@@ -12090,9 +12159,11 @@
       <c r="FQ65" s="4"/>
       <c r="FR65" s="9"/>
       <c r="FS65" s="9"/>
+      <c r="FU65"/>
       <c r="FV65"/>
+      <c r="FW65"/>
     </row>
-    <row r="66" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>1</v>
       </c>
@@ -12616,11 +12687,16 @@
         <v>7.7150759459390343</v>
       </c>
       <c r="FS66" s="11">
-        <v>6.8275183225073164</v>
-      </c>
+        <v>6.7851118468915388</v>
+      </c>
+      <c r="FT66" s="11">
+        <v>5.5097719950694284</v>
+      </c>
+      <c r="FU66"/>
       <c r="FV66"/>
+      <c r="FW66"/>
     </row>
-    <row r="67" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>2</v>
       </c>
@@ -13144,11 +13220,16 @@
         <v>21.583952465986258</v>
       </c>
       <c r="FS67" s="11">
-        <v>10.657843504192272</v>
-      </c>
+        <v>10.666669079881245</v>
+      </c>
+      <c r="FT67" s="11">
+        <v>7.5973847843585389</v>
+      </c>
+      <c r="FU67"/>
       <c r="FV67"/>
+      <c r="FW67"/>
     </row>
-    <row r="68" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>3</v>
       </c>
@@ -13672,11 +13753,16 @@
         <v>8.520991494478551</v>
       </c>
       <c r="FS68" s="11">
-        <v>0.79937476882894032</v>
-      </c>
+        <v>1.4741924447766053</v>
+      </c>
+      <c r="FT68" s="11">
+        <v>-0.82847032874462911</v>
+      </c>
+      <c r="FU68"/>
       <c r="FV68"/>
+      <c r="FW68"/>
     </row>
-    <row r="69" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>4</v>
       </c>
@@ -14200,11 +14286,16 @@
         <v>9.8714297907661006</v>
       </c>
       <c r="FS69" s="11">
-        <v>4.1122649187381768</v>
-      </c>
+        <v>4.3316757846278051</v>
+      </c>
+      <c r="FT69" s="11">
+        <v>8.2029618312790689</v>
+      </c>
+      <c r="FU69"/>
       <c r="FV69"/>
+      <c r="FW69"/>
     </row>
-    <row r="70" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>5</v>
       </c>
@@ -14728,11 +14819,16 @@
         <v>14.707435060697321</v>
       </c>
       <c r="FS70" s="11">
-        <v>0.87443085699105438</v>
-      </c>
+        <v>1.4761820532143304</v>
+      </c>
+      <c r="FT70" s="11">
+        <v>3.6182152930054343</v>
+      </c>
+      <c r="FU70"/>
       <c r="FV70"/>
+      <c r="FW70"/>
     </row>
-    <row r="71" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="B71" s="11"/>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
@@ -14907,9 +15003,12 @@
       <c r="FQ71" s="11"/>
       <c r="FR71" s="11"/>
       <c r="FS71" s="11"/>
+      <c r="FT71" s="11"/>
+      <c r="FU71"/>
       <c r="FV71"/>
+      <c r="FW71"/>
     </row>
-    <row r="72" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="B72" s="11"/>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
@@ -15084,9 +15183,12 @@
       <c r="FQ72" s="11"/>
       <c r="FR72" s="11"/>
       <c r="FS72" s="11"/>
+      <c r="FT72" s="11"/>
+      <c r="FU72"/>
       <c r="FV72"/>
+      <c r="FW72"/>
     </row>
-    <row r="73" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>10</v>
       </c>
@@ -15610,23 +15712,36 @@
         <v>7.5656166312838167</v>
       </c>
       <c r="FS73" s="11">
-        <v>7.2414976519282703</v>
-      </c>
+        <v>7.2436961834564784</v>
+      </c>
+      <c r="FT73" s="11">
+        <v>4.8501323885663368</v>
+      </c>
+      <c r="FU73"/>
       <c r="FV73"/>
+      <c r="FW73"/>
     </row>
-    <row r="74" spans="1:178" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:179" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="FU74"/>
       <c r="FV74"/>
+      <c r="FW74"/>
     </row>
-    <row r="75" spans="1:178" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:179" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="FU75"/>
       <c r="FV75"/>
+      <c r="FW75"/>
     </row>
-    <row r="76" spans="1:178" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:179" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="FU76"/>
       <c r="FV76"/>
+      <c r="FW76"/>
     </row>
-    <row r="77" spans="1:178" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:179" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="FU77"/>
       <c r="FV77"/>
+      <c r="FW77"/>
     </row>
-    <row r="78" spans="1:178" ht="7.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:179" ht="7.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
@@ -15800,65 +15915,88 @@
       <c r="FP78" s="8"/>
       <c r="FR78" s="8"/>
       <c r="FS78" s="8"/>
+      <c r="FT78" s="8"/>
+      <c r="FU78"/>
       <c r="FV78"/>
+      <c r="FW78"/>
     </row>
-    <row r="79" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>0</v>
       </c>
       <c r="FM79" s="4"/>
       <c r="FQ79" s="4"/>
+      <c r="FU79"/>
       <c r="FV79"/>
+      <c r="FW79"/>
     </row>
-    <row r="80" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="FU80"/>
       <c r="FV80"/>
+      <c r="FW80"/>
     </row>
-    <row r="81" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:179" ht="15" x14ac:dyDescent="0.25">
+      <c r="FU81"/>
       <c r="FV81"/>
+      <c r="FW81"/>
     </row>
-    <row r="82" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="FU82"/>
       <c r="FV82"/>
+      <c r="FW82"/>
     </row>
-    <row r="83" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="FU83"/>
       <c r="FV83"/>
+      <c r="FW83"/>
     </row>
-    <row r="84" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="FU84"/>
       <c r="FV84"/>
+      <c r="FW84"/>
     </row>
-    <row r="85" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:179" ht="15" x14ac:dyDescent="0.25">
+      <c r="FU85"/>
       <c r="FV85"/>
+      <c r="FW85"/>
     </row>
-    <row r="86" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="FU86"/>
       <c r="FV86"/>
+      <c r="FW86"/>
     </row>
-    <row r="87" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>40</v>
       </c>
+      <c r="FU87"/>
       <c r="FV87"/>
+      <c r="FW87"/>
     </row>
-    <row r="88" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="FU88"/>
       <c r="FV88"/>
+      <c r="FW88"/>
     </row>
-    <row r="89" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="B89" s="8"/>
       <c r="C89" s="8"/>
       <c r="F89" s="8"/>
@@ -15941,9 +16079,11 @@
       <c r="FC89" s="8"/>
       <c r="FF89" s="8"/>
       <c r="FG89" s="8"/>
+      <c r="FU89"/>
       <c r="FV89"/>
+      <c r="FW89"/>
     </row>
-    <row r="90" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="5" t="s">
         <v>42</v>
@@ -16207,9 +16347,12 @@
         <v>85</v>
       </c>
       <c r="FS90" s="5"/>
+      <c r="FT90" s="5"/>
+      <c r="FU90"/>
       <c r="FV90"/>
+      <c r="FW90"/>
     </row>
-    <row r="91" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>14</v>
       </c>
@@ -16735,9 +16878,14 @@
       <c r="FS91" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="FT91" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="FU91"/>
       <c r="FV91"/>
+      <c r="FW91"/>
     </row>
-    <row r="92" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
       <c r="D92" s="9"/>
@@ -16910,9 +17058,11 @@
       <c r="FQ92" s="4"/>
       <c r="FR92" s="9"/>
       <c r="FS92" s="9"/>
+      <c r="FU92"/>
       <c r="FV92"/>
+      <c r="FW92"/>
     </row>
-    <row r="93" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>1</v>
       </c>
@@ -17436,11 +17586,16 @@
         <v>5.2936401126761012</v>
       </c>
       <c r="FS93" s="11">
-        <v>5.4514379593826305</v>
-      </c>
+        <v>5.3161507759349718</v>
+      </c>
+      <c r="FT93" s="11">
+        <v>4.054943874924021</v>
+      </c>
+      <c r="FU93"/>
       <c r="FV93"/>
+      <c r="FW93"/>
     </row>
-    <row r="94" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>2</v>
       </c>
@@ -17964,11 +18119,16 @@
         <v>18.693834311372257</v>
       </c>
       <c r="FS94" s="11">
-        <v>8.7061776566054334</v>
-      </c>
+        <v>8.7145001406101272</v>
+      </c>
+      <c r="FT94" s="11">
+        <v>5.7591380394603533</v>
+      </c>
+      <c r="FU94"/>
       <c r="FV94"/>
+      <c r="FW94"/>
     </row>
-    <row r="95" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>3</v>
       </c>
@@ -18492,11 +18652,16 @@
         <v>4.763494983860511</v>
       </c>
       <c r="FS95" s="11">
-        <v>0.58975020723219984</v>
-      </c>
+        <v>1.162331894472743</v>
+      </c>
+      <c r="FT95" s="11">
+        <v>-2.8095463351609169</v>
+      </c>
+      <c r="FU95"/>
       <c r="FV95"/>
+      <c r="FW95"/>
     </row>
-    <row r="96" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>4</v>
       </c>
@@ -19020,11 +19185,16 @@
         <v>7.0863742590254475</v>
       </c>
       <c r="FS96" s="11">
-        <v>4.4110417694631678</v>
-      </c>
+        <v>4.7286889141274173</v>
+      </c>
+      <c r="FT96" s="11">
+        <v>6.9824628738995358</v>
+      </c>
+      <c r="FU96"/>
       <c r="FV96"/>
+      <c r="FW96"/>
     </row>
-    <row r="97" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>5</v>
       </c>
@@ -19548,11 +19718,16 @@
         <v>10.307723082650028</v>
       </c>
       <c r="FS97" s="11">
-        <v>2.859215398799563</v>
-      </c>
+        <v>3.4690342255737221</v>
+      </c>
+      <c r="FT97" s="11">
+        <v>2.6419035849809802</v>
+      </c>
+      <c r="FU97"/>
       <c r="FV97"/>
+      <c r="FW97"/>
     </row>
-    <row r="98" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="B98" s="11"/>
       <c r="C98" s="11"/>
       <c r="D98" s="11"/>
@@ -19727,9 +19902,12 @@
       <c r="FQ98" s="11"/>
       <c r="FR98" s="11"/>
       <c r="FS98" s="11"/>
+      <c r="FT98" s="11"/>
+      <c r="FU98"/>
       <c r="FV98"/>
+      <c r="FW98"/>
     </row>
-    <row r="99" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="B99" s="11"/>
       <c r="C99" s="11"/>
       <c r="D99" s="11"/>
@@ -19904,9 +20082,12 @@
       <c r="FQ99" s="11"/>
       <c r="FR99" s="11"/>
       <c r="FS99" s="11"/>
+      <c r="FT99" s="11"/>
+      <c r="FU99"/>
       <c r="FV99"/>
+      <c r="FW99"/>
     </row>
-    <row r="100" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
         <v>10</v>
       </c>
@@ -20430,23 +20611,36 @@
         <v>5.3793620546446448</v>
       </c>
       <c r="FS100" s="11">
-        <v>5.4759513968919435</v>
-      </c>
+        <v>5.4874450057838402</v>
+      </c>
+      <c r="FT100" s="11">
+        <v>4.0025977978986447</v>
+      </c>
+      <c r="FU100"/>
       <c r="FV100"/>
+      <c r="FW100"/>
     </row>
-    <row r="101" spans="1:178" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:179" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="FU101"/>
       <c r="FV101"/>
+      <c r="FW101"/>
     </row>
-    <row r="102" spans="1:178" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:179" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="FU102"/>
       <c r="FV102"/>
+      <c r="FW102"/>
     </row>
-    <row r="103" spans="1:178" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:179" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="FU103"/>
       <c r="FV103"/>
+      <c r="FW103"/>
     </row>
-    <row r="104" spans="1:178" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:179" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="FU104"/>
       <c r="FV104"/>
+      <c r="FW104"/>
     </row>
-    <row r="105" spans="1:178" ht="7.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:179" ht="7.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="8"/>
       <c r="B105" s="8"/>
       <c r="C105" s="8"/>
@@ -20618,9 +20812,11 @@
       <c r="FO105" s="8"/>
       <c r="FR105" s="8"/>
       <c r="FS105" s="8"/>
+      <c r="FU105"/>
       <c r="FV105"/>
+      <c r="FW105"/>
     </row>
-    <row r="106" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>0</v>
       </c>
@@ -20628,48 +20824,55 @@
       <c r="FM106" s="4"/>
       <c r="FP106" s="4"/>
       <c r="FQ106" s="4"/>
+      <c r="FT106" s="4"/>
+      <c r="FU106"/>
       <c r="FV106"/>
+      <c r="FW106"/>
     </row>
-    <row r="107" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="FU107"/>
       <c r="FV107"/>
+      <c r="FW107"/>
     </row>
-    <row r="108" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:179" ht="15" x14ac:dyDescent="0.25">
+      <c r="FU108"/>
       <c r="FV108"/>
+      <c r="FW108"/>
     </row>
-    <row r="109" spans="1:178" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="110" spans="1:178" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:178" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="113" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="115" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="117" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A117" s="4"/>
       <c r="B117" s="5">
         <v>1981</v>
@@ -20939,8 +21142,9 @@
         <v>2025</v>
       </c>
       <c r="FW117" s="5"/>
+      <c r="FX117" s="5"/>
     </row>
-    <row r="118" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>14</v>
       </c>
@@ -21478,8 +21682,11 @@
       <c r="FW118" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="FX118" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="120" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>1</v>
       </c>
@@ -22015,10 +22222,13 @@
         <v>78.266835488909905</v>
       </c>
       <c r="FW120" s="11">
-        <v>72.195506756124757</v>
+        <v>72.165368431976617</v>
+      </c>
+      <c r="FX120" s="11">
+        <v>79.134395812920346</v>
       </c>
     </row>
-    <row r="121" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>2</v>
       </c>
@@ -22554,10 +22764,13 @@
         <v>14.832449406055986</v>
       </c>
       <c r="FW121" s="11">
-        <v>16.898271938498279</v>
+        <v>16.899273221406773</v>
+      </c>
+      <c r="FX121" s="11">
+        <v>15.49125793977201</v>
       </c>
     </row>
-    <row r="122" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>3</v>
       </c>
@@ -23093,10 +23306,13 @@
         <v>22.367773115632438</v>
       </c>
       <c r="FW122" s="11">
-        <v>26.067899390180884</v>
+        <v>26.241877169817712</v>
+      </c>
+      <c r="FX122" s="11">
+        <v>22.440834454219093</v>
       </c>
     </row>
-    <row r="123" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>4</v>
       </c>
@@ -23632,10 +23848,13 @@
         <v>28.394731713738615</v>
       </c>
       <c r="FW123" s="11">
-        <v>24.243610415610018</v>
+        <v>24.294204440205284</v>
+      </c>
+      <c r="FX123" s="11">
+        <v>28.815789278701864</v>
       </c>
     </row>
-    <row r="124" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>5</v>
       </c>
@@ -24171,10 +24390,13 @@
         <v>43.275897413015002</v>
       </c>
       <c r="FW124" s="11">
-        <v>38.732943598349713</v>
+        <v>38.963200353955848</v>
+      </c>
+      <c r="FX124" s="11">
+        <v>45.204026300361775</v>
       </c>
     </row>
-    <row r="125" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:180" x14ac:dyDescent="0.2">
       <c r="B125" s="11"/>
       <c r="C125" s="11"/>
       <c r="D125" s="11"/>
@@ -24353,8 +24575,9 @@
       <c r="FU125" s="11"/>
       <c r="FV125" s="11"/>
       <c r="FW125" s="11"/>
+      <c r="FX125" s="11"/>
     </row>
-    <row r="126" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:180" x14ac:dyDescent="0.2">
       <c r="B126" s="11"/>
       <c r="C126" s="11"/>
       <c r="D126" s="11"/>
@@ -24533,8 +24756,9 @@
       <c r="FU126" s="11"/>
       <c r="FV126" s="11"/>
       <c r="FW126" s="11"/>
+      <c r="FX126" s="11"/>
     </row>
-    <row r="127" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A127" s="7" t="s">
         <v>10</v>
       </c>
@@ -25072,28 +25296,31 @@
       <c r="FW127" s="11">
         <v>100</v>
       </c>
+      <c r="FX127" s="11">
+        <v>100</v>
+      </c>
     </row>
-    <row r="128" spans="1:179" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:180" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B128" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:179" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B129" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:179" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B130" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:179" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B131" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:179" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:180" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="8"/>
       <c r="B132" s="8"/>
       <c r="C132" s="8"/>
@@ -25273,43 +25500,44 @@
       <c r="FU132" s="8"/>
       <c r="FV132" s="8"/>
       <c r="FW132" s="8"/>
+      <c r="FX132" s="8"/>
     </row>
-    <row r="133" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="137" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="140" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="141" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="142" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="144" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A144" s="4"/>
       <c r="B144" s="5">
         <v>1981</v>
@@ -25579,8 +25807,9 @@
         <v>2025</v>
       </c>
       <c r="FW144" s="5"/>
+      <c r="FX144" s="5"/>
     </row>
-    <row r="145" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>14</v>
       </c>
@@ -26118,8 +26347,11 @@
       <c r="FW145" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="FX145" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="147" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>1</v>
       </c>
@@ -26655,10 +26887,13 @@
         <v>74.333251043763042</v>
       </c>
       <c r="FW147" s="11">
-        <v>67.757295719726002</v>
+        <v>67.662994445686621</v>
+      </c>
+      <c r="FX147" s="11">
+        <v>72.946591718413174</v>
       </c>
     </row>
-    <row r="148" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>2</v>
       </c>
@@ -27194,10 +27429,13 @@
         <v>15.908480539482833</v>
       </c>
       <c r="FW148" s="11">
-        <v>17.456210000199128</v>
+        <v>17.455644313752238</v>
+      </c>
+      <c r="FX148" s="11">
+        <v>14.961405517338658</v>
       </c>
     </row>
-    <row r="149" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>3</v>
       </c>
@@ -27733,10 +27971,13 @@
         <v>21.999093315322995</v>
       </c>
       <c r="FW149" s="11">
-        <v>26.020069235360555</v>
+        <v>26.165330682204175</v>
+      </c>
+      <c r="FX149" s="11">
+        <v>21.453780108947377</v>
       </c>
     </row>
-    <row r="150" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>4</v>
       </c>
@@ -28272,10 +28513,13 @@
         <v>29.050845381654099</v>
       </c>
       <c r="FW150" s="11">
-        <v>26.419582608446479</v>
+        <v>26.497070895592621</v>
+      </c>
+      <c r="FX150" s="11">
+        <v>30.098054814796569</v>
       </c>
     </row>
-    <row r="151" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>5</v>
       </c>
@@ -28811,10 +29055,13 @@
         <v>40.843965488437576</v>
       </c>
       <c r="FW151" s="11">
-        <v>37.249158550380088</v>
+        <v>37.465914070660759</v>
+      </c>
+      <c r="FX151" s="11">
+        <v>39.934871547707324</v>
       </c>
     </row>
-    <row r="152" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:180" x14ac:dyDescent="0.2">
       <c r="B152" s="11"/>
       <c r="C152" s="11"/>
       <c r="D152" s="11"/>
@@ -28993,8 +29240,9 @@
       <c r="FU152" s="11"/>
       <c r="FV152" s="11"/>
       <c r="FW152" s="11"/>
+      <c r="FX152" s="11"/>
     </row>
-    <row r="153" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:180" x14ac:dyDescent="0.2">
       <c r="B153" s="11"/>
       <c r="C153" s="11"/>
       <c r="D153" s="11"/>
@@ -29173,8 +29421,9 @@
       <c r="FU153" s="11"/>
       <c r="FV153" s="11"/>
       <c r="FW153" s="11"/>
+      <c r="FX153" s="11"/>
     </row>
-    <row r="154" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A154" s="7" t="s">
         <v>10</v>
       </c>
@@ -29712,12 +29961,15 @@
       <c r="FW154" s="11">
         <v>100</v>
       </c>
+      <c r="FX154" s="11">
+        <v>100</v>
+      </c>
     </row>
-    <row r="155" spans="1:179" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="156" spans="1:179" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="157" spans="1:179" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="158" spans="1:179" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" spans="1:179" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:180" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" spans="1:180" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" spans="1:180" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" spans="1:180" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" spans="1:180" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="8"/>
       <c r="B159" s="8"/>
       <c r="C159" s="8"/>
@@ -29897,43 +30149,44 @@
       <c r="FU159" s="8"/>
       <c r="FV159" s="8"/>
       <c r="FW159" s="8"/>
+      <c r="FX159" s="8"/>
     </row>
-    <row r="160" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="164" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="165" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="167" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="168" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="169" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="171" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A171" s="4"/>
       <c r="B171" s="5">
         <v>1981</v>
@@ -30203,8 +30456,9 @@
         <v>2025</v>
       </c>
       <c r="FW171" s="5"/>
+      <c r="FX171" s="5"/>
     </row>
-    <row r="172" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>13</v>
       </c>
@@ -30742,8 +30996,11 @@
       <c r="FW172" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="FX172" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="174" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A174" s="12" t="s">
         <v>36</v>
       </c>
@@ -31279,10 +31536,13 @@
         <v>626803.95607463922</v>
       </c>
       <c r="FW174" s="6">
-        <v>563892.36464639392</v>
+        <v>563588.84775933588</v>
+      </c>
+      <c r="FX174" s="6">
+        <v>526613.31456431362</v>
       </c>
     </row>
-    <row r="175" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A175" s="12" t="s">
         <v>37</v>
       </c>
@@ -31818,10 +32078,13 @@
         <v>1854773.7098244908</v>
       </c>
       <c r="FW175" s="6">
-        <v>1981256.3212099909</v>
+        <v>1981339.3138687818</v>
+      </c>
+      <c r="FX175" s="6">
+        <v>1549050.7836458907</v>
       </c>
     </row>
-    <row r="176" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A176" s="12" t="s">
         <v>38</v>
       </c>
@@ -32357,10 +32620,13 @@
         <v>4100509.1894691316</v>
       </c>
       <c r="FW176" s="6">
-        <v>4419943.7260055812</v>
+        <v>4420307.0398777789</v>
+      </c>
+      <c r="FX176" s="6">
+        <v>4482314.4179834872</v>
       </c>
     </row>
-    <row r="177" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A177" s="14"/>
       <c r="B177" s="6"/>
       <c r="C177" s="6"/>
@@ -32540,8 +32806,9 @@
       <c r="FU177" s="6"/>
       <c r="FV177" s="6"/>
       <c r="FW177" s="6"/>
+      <c r="FX177" s="6"/>
     </row>
-    <row r="178" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>10</v>
       </c>
@@ -33077,10 +33344,13 @@
         <v>6582086.8553682622</v>
       </c>
       <c r="FW178" s="6">
-        <v>6965092.4118619654</v>
+        <v>6965235.2015058966</v>
+      </c>
+      <c r="FX178" s="6">
+        <v>6557978.5161936916</v>
       </c>
     </row>
-    <row r="179" spans="1:179" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:180" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="FB179" s="1">
         <v>20558.222744577564</v>
       </c>
@@ -33088,8 +33358,8 @@
         <v>-24370.119758612476</v>
       </c>
     </row>
-    <row r="180" spans="1:179" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="181" spans="1:179" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:180" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="181" spans="1:180" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="FB181" s="1">
         <v>4422950.8840171499</v>
       </c>
@@ -33097,8 +33367,8 @@
         <v>4857262.3839106075</v>
       </c>
     </row>
-    <row r="182" spans="1:179" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="183" spans="1:179" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:180" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" spans="1:180" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="8"/>
       <c r="B183" s="8"/>
       <c r="C183" s="8"/>
@@ -33278,49 +33548,50 @@
       <c r="FU183" s="8"/>
       <c r="FV183" s="8"/>
       <c r="FW183" s="8"/>
+      <c r="FX183" s="8"/>
     </row>
-    <row r="184" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="188" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="189" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="190" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A190" s="1"/>
     </row>
-    <row r="191" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="192" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="193" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="194" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A194" s="1"/>
     </row>
-    <row r="195" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A195" s="4"/>
       <c r="B195" s="5">
         <v>1981</v>
@@ -33590,8 +33861,9 @@
         <v>2025</v>
       </c>
       <c r="FW195" s="5"/>
+      <c r="FX195" s="5"/>
     </row>
-    <row r="196" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
         <v>13</v>
       </c>
@@ -34129,8 +34401,11 @@
       <c r="FW196" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="FX196" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="198" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A198" s="12" t="s">
         <v>36</v>
       </c>
@@ -34666,10 +34941,13 @@
         <v>456879.88893348817</v>
       </c>
       <c r="FW198" s="6">
-        <v>436434.86507390434</v>
+        <v>436443.61944668175</v>
+      </c>
+      <c r="FX198" s="6">
+        <v>410864.28179950779</v>
       </c>
     </row>
-    <row r="199" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A199" s="12" t="s">
         <v>37</v>
       </c>
@@ -35205,10 +35483,13 @@
         <v>1617032.2826460856</v>
       </c>
       <c r="FW199" s="6">
-        <v>1711441.7591528599</v>
+        <v>1710944.93384886</v>
+      </c>
+      <c r="FX199" s="6">
+        <v>1430415.750393182</v>
       </c>
     </row>
-    <row r="200" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A200" s="12" t="s">
         <v>38</v>
       </c>
@@ -35744,10 +36025,13 @@
         <v>3401165.5327608078</v>
       </c>
       <c r="FW200" s="6">
-        <v>3694523.5609110193</v>
+        <v>3695648.2723449231</v>
+      </c>
+      <c r="FX200" s="6">
+        <v>3687554.5667276606</v>
       </c>
     </row>
-    <row r="201" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A201" s="14"/>
       <c r="B201" s="6"/>
       <c r="C201" s="6"/>
@@ -35927,8 +36211,9 @@
       <c r="FU201" s="6"/>
       <c r="FV201" s="6"/>
       <c r="FW201" s="6"/>
+      <c r="FX201" s="6"/>
     </row>
-    <row r="202" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>10</v>
       </c>
@@ -36464,10 +36749,13 @@
         <v>5475077.7043403815</v>
       </c>
       <c r="FW202" s="6">
-        <v>5842400.1851377841</v>
+        <v>5843036.8256404642</v>
+      </c>
+      <c r="FX202" s="6">
+        <v>5528834.5989203509</v>
       </c>
     </row>
-    <row r="203" spans="1:179" s="13" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:180" s="13" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="1"/>
       <c r="FB203" s="13">
         <v>20558.222744577564</v>
@@ -36485,8 +36773,9 @@
       <c r="FT203" s="1"/>
       <c r="FU203" s="1"/>
       <c r="FW203" s="1"/>
+      <c r="FX203" s="1"/>
     </row>
-    <row r="204" spans="1:179" s="13" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:180" s="13" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="1"/>
       <c r="FK204" s="1"/>
       <c r="FL204" s="1"/>
@@ -36498,8 +36787,9 @@
       <c r="FT204" s="1"/>
       <c r="FU204" s="1"/>
       <c r="FW204" s="1"/>
+      <c r="FX204" s="1"/>
     </row>
-    <row r="205" spans="1:179" s="13" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:180" s="13" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="1"/>
       <c r="FB205" s="13">
         <v>4422950.8840171499</v>
@@ -36517,8 +36807,9 @@
       <c r="FT205" s="1"/>
       <c r="FU205" s="1"/>
       <c r="FW205" s="1"/>
+      <c r="FX205" s="1"/>
     </row>
-    <row r="206" spans="1:179" s="13" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:180" s="13" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="1"/>
       <c r="FK206" s="1"/>
       <c r="FL206" s="1"/>
@@ -36530,8 +36821,9 @@
       <c r="FT206" s="1"/>
       <c r="FU206" s="1"/>
       <c r="FW206" s="1"/>
+      <c r="FX206" s="1"/>
     </row>
-    <row r="207" spans="1:179" s="13" customFormat="1" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:180" s="13" customFormat="1" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="8"/>
       <c r="B207" s="8"/>
       <c r="C207" s="8"/>
@@ -36711,46 +37003,62 @@
       <c r="FU207" s="8"/>
       <c r="FV207" s="8"/>
       <c r="FW207" s="8"/>
+      <c r="FX207" s="8"/>
     </row>
-    <row r="208" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:178" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="212" spans="1:178" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="213" spans="1:178" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="215" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:180" ht="15" x14ac:dyDescent="0.25">
+      <c r="FU214"/>
+      <c r="FV214"/>
+      <c r="FW214"/>
+      <c r="FX214"/>
+    </row>
+    <row r="215" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>30</v>
       </c>
       <c r="FU215"/>
+      <c r="FV215"/>
+      <c r="FW215"/>
+      <c r="FX215"/>
     </row>
-    <row r="216" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
         <v>40</v>
       </c>
       <c r="FU216"/>
+      <c r="FV216"/>
+      <c r="FW216"/>
+      <c r="FX216"/>
     </row>
-    <row r="217" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="FU217"/>
       <c r="FV217"/>
+      <c r="FW217"/>
+      <c r="FX217"/>
     </row>
-    <row r="218" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="B218" s="8"/>
       <c r="C218" s="8"/>
       <c r="F218" s="8"/>
@@ -36835,9 +37143,13 @@
       <c r="FG218" s="8"/>
       <c r="FL218" s="8"/>
       <c r="FP218" s="8"/>
+      <c r="FT218" s="8"/>
+      <c r="FU218"/>
       <c r="FV218"/>
+      <c r="FW218"/>
+      <c r="FX218"/>
     </row>
-    <row r="219" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A219" s="4"/>
       <c r="B219" s="5" t="s">
         <v>42</v>
@@ -37101,9 +37413,13 @@
         <v>85</v>
       </c>
       <c r="FS219" s="5"/>
+      <c r="FT219" s="5"/>
+      <c r="FU219"/>
       <c r="FV219"/>
+      <c r="FW219"/>
+      <c r="FX219"/>
     </row>
-    <row r="220" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>13</v>
       </c>
@@ -37629,9 +37945,15 @@
       <c r="FS220" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="FT220" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="FU220"/>
       <c r="FV220"/>
+      <c r="FW220"/>
+      <c r="FX220"/>
     </row>
-    <row r="221" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="B221" s="9"/>
       <c r="F221" s="9"/>
       <c r="J221" s="9"/>
@@ -37683,9 +38005,13 @@
       <c r="FQ221" s="4"/>
       <c r="FR221" s="9"/>
       <c r="FS221" s="9"/>
+      <c r="FT221" s="4"/>
+      <c r="FU221"/>
       <c r="FV221"/>
+      <c r="FW221"/>
+      <c r="FX221"/>
     </row>
-    <row r="222" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A222" s="12" t="s">
         <v>36</v>
       </c>
@@ -38209,11 +38535,17 @@
         <v>2.0742119320947552</v>
       </c>
       <c r="FS222" s="11">
-        <v>5.0970879980940964</v>
-      </c>
+        <v>5.0405191509382234</v>
+      </c>
+      <c r="FT222" s="11">
+        <v>-3.9142455240438068</v>
+      </c>
+      <c r="FU222"/>
       <c r="FV222"/>
+      <c r="FW222"/>
+      <c r="FX222"/>
     </row>
-    <row r="223" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A223" s="12" t="s">
         <v>37</v>
       </c>
@@ -38737,11 +39069,17 @@
         <v>6.8769584626979992</v>
       </c>
       <c r="FS223" s="11">
-        <v>4.4391109504121573</v>
-      </c>
+        <v>4.443485790460258</v>
+      </c>
+      <c r="FT223" s="11">
+        <v>1.339452890673769</v>
+      </c>
+      <c r="FU223"/>
       <c r="FV223"/>
+      <c r="FW223"/>
+      <c r="FX223"/>
     </row>
-    <row r="224" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A224" s="12" t="s">
         <v>38</v>
       </c>
@@ -39265,11 +39603,17 @@
         <v>8.777192951259309</v>
       </c>
       <c r="FS224" s="11">
-        <v>8.8338463991900653</v>
-      </c>
+        <v>8.8427924058844098</v>
+      </c>
+      <c r="FT224" s="11">
+        <v>7.2842754538257992</v>
+      </c>
+      <c r="FU224"/>
       <c r="FV224"/>
+      <c r="FW224"/>
+      <c r="FX224"/>
     </row>
-    <row r="225" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A225" s="14"/>
       <c r="B225" s="11"/>
       <c r="C225" s="11"/>
@@ -39445,9 +39789,13 @@
       <c r="FQ225" s="11"/>
       <c r="FR225" s="11"/>
       <c r="FS225" s="11"/>
+      <c r="FT225" s="11"/>
+      <c r="FU225"/>
       <c r="FV225"/>
+      <c r="FW225"/>
+      <c r="FX225"/>
     </row>
-    <row r="226" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>10</v>
       </c>
@@ -39971,11 +40319,17 @@
         <v>7.5656166312838167</v>
       </c>
       <c r="FS226" s="11">
-        <v>7.2414976519282703</v>
-      </c>
+        <v>7.2436961834564784</v>
+      </c>
+      <c r="FT226" s="11">
+        <v>4.8501323885663368</v>
+      </c>
+      <c r="FU226"/>
       <c r="FV226"/>
+      <c r="FW226"/>
+      <c r="FX226"/>
     </row>
-    <row r="227" spans="1:178" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B227" s="16"/>
       <c r="C227" s="16"/>
       <c r="D227" s="16"/>
@@ -40150,9 +40504,12 @@
       <c r="FO227" s="16"/>
       <c r="FR227" s="16"/>
       <c r="FS227" s="16"/>
+      <c r="FU227"/>
       <c r="FV227"/>
+      <c r="FW227"/>
+      <c r="FX227"/>
     </row>
-    <row r="228" spans="1:178" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B228" s="16"/>
       <c r="C228" s="16"/>
       <c r="D228" s="16"/>
@@ -40327,9 +40684,12 @@
       <c r="FO228" s="16"/>
       <c r="FR228" s="16"/>
       <c r="FS228" s="16"/>
+      <c r="FU228"/>
       <c r="FV228"/>
+      <c r="FW228"/>
+      <c r="FX228"/>
     </row>
-    <row r="229" spans="1:178" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B229" s="16"/>
       <c r="C229" s="16"/>
       <c r="D229" s="16"/>
@@ -40510,18 +40870,24 @@
         <v>14.6558695901769</v>
       </c>
       <c r="FS229" s="16"/>
+      <c r="FU229"/>
       <c r="FV229"/>
+      <c r="FW229"/>
+      <c r="FX229"/>
     </row>
-    <row r="230" spans="1:178" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="EX230" s="1" t="e">
         <v>#DIV/0!</v>
       </c>
       <c r="EY230" s="1" t="e">
         <v>#DIV/0!</v>
       </c>
+      <c r="FU230"/>
       <c r="FV230"/>
+      <c r="FW230"/>
+      <c r="FX230"/>
     </row>
-    <row r="231" spans="1:178" ht="7.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:180" ht="7.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="8"/>
       <c r="B231" s="8"/>
       <c r="C231" s="8"/>
@@ -40693,9 +41059,12 @@
       <c r="FO231" s="8"/>
       <c r="FR231" s="8"/>
       <c r="FS231" s="8"/>
+      <c r="FU231"/>
       <c r="FV231"/>
+      <c r="FW231"/>
+      <c r="FX231"/>
     </row>
-    <row r="232" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>0</v>
       </c>
@@ -40703,54 +41072,85 @@
       <c r="FM232" s="4"/>
       <c r="FP232" s="4"/>
       <c r="FQ232" s="4"/>
+      <c r="FT232" s="4"/>
+      <c r="FU232"/>
       <c r="FV232"/>
+      <c r="FW232"/>
+      <c r="FX232"/>
     </row>
-    <row r="233" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:180" ht="15" x14ac:dyDescent="0.25">
+      <c r="FU233"/>
       <c r="FV233"/>
+      <c r="FW233"/>
+      <c r="FX233"/>
     </row>
-    <row r="234" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:180" ht="15" x14ac:dyDescent="0.25">
+      <c r="FU234"/>
       <c r="FV234"/>
+      <c r="FW234"/>
+      <c r="FX234"/>
     </row>
-    <row r="235" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="FU235"/>
       <c r="FV235"/>
+      <c r="FW235"/>
+      <c r="FX235"/>
     </row>
-    <row r="236" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="FU236"/>
       <c r="FV236"/>
+      <c r="FW236"/>
+      <c r="FX236"/>
     </row>
-    <row r="237" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="FU237"/>
       <c r="FV237"/>
+      <c r="FW237"/>
+      <c r="FX237"/>
     </row>
-    <row r="238" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:180" ht="15" x14ac:dyDescent="0.25">
+      <c r="FU238"/>
       <c r="FV238"/>
+      <c r="FW238"/>
+      <c r="FX238"/>
     </row>
-    <row r="239" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="FU239"/>
       <c r="FV239"/>
+      <c r="FW239"/>
+      <c r="FX239"/>
     </row>
-    <row r="240" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A240" s="3" t="s">
         <v>40</v>
       </c>
+      <c r="FU240"/>
       <c r="FV240"/>
+      <c r="FW240"/>
+      <c r="FX240"/>
     </row>
-    <row r="241" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="FU241"/>
       <c r="FV241"/>
+      <c r="FW241"/>
+      <c r="FX241"/>
     </row>
-    <row r="242" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="B242" s="8"/>
       <c r="C242" s="8"/>
       <c r="F242" s="8"/>
@@ -40835,9 +41235,13 @@
       <c r="FG242" s="8"/>
       <c r="FL242" s="8"/>
       <c r="FP242" s="8"/>
+      <c r="FT242" s="8"/>
+      <c r="FU242"/>
       <c r="FV242"/>
+      <c r="FW242"/>
+      <c r="FX242"/>
     </row>
-    <row r="243" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A243" s="4"/>
       <c r="B243" s="5" t="s">
         <v>42</v>
@@ -41101,9 +41505,13 @@
         <v>85</v>
       </c>
       <c r="FS243" s="5"/>
+      <c r="FT243" s="5"/>
+      <c r="FU243"/>
       <c r="FV243"/>
+      <c r="FW243"/>
+      <c r="FX243"/>
     </row>
-    <row r="244" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>13</v>
       </c>
@@ -41629,9 +42037,15 @@
       <c r="FS244" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="FT244" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="FU244"/>
       <c r="FV244"/>
+      <c r="FW244"/>
+      <c r="FX244"/>
     </row>
-    <row r="245" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="B245" s="9"/>
       <c r="F245" s="9"/>
       <c r="J245" s="9"/>
@@ -41681,9 +42095,12 @@
       <c r="FQ245" s="4"/>
       <c r="FR245" s="9"/>
       <c r="FS245" s="9"/>
+      <c r="FU245"/>
       <c r="FV245"/>
+      <c r="FW245"/>
+      <c r="FX245"/>
     </row>
-    <row r="246" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A246" s="12" t="s">
         <v>36</v>
       </c>
@@ -42207,11 +42624,17 @@
         <v>2.2332920366867199</v>
       </c>
       <c r="FS246" s="11">
-        <v>6.954186965622327</v>
-      </c>
+        <v>6.9563323414796088</v>
+      </c>
+      <c r="FT246" s="11">
+        <v>2.8463855572208985</v>
+      </c>
+      <c r="FU246"/>
       <c r="FV246"/>
+      <c r="FW246"/>
+      <c r="FX246"/>
     </row>
-    <row r="247" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A247" s="12" t="s">
         <v>37</v>
       </c>
@@ -42735,11 +43158,17 @@
         <v>4.5885477670543793</v>
       </c>
       <c r="FS247" s="11">
-        <v>2.140783191066788</v>
-      </c>
+        <v>2.1111320940380409</v>
+      </c>
+      <c r="FT247" s="11">
+        <v>0.70692392551127625</v>
+      </c>
+      <c r="FU247"/>
       <c r="FV247"/>
+      <c r="FW247"/>
+      <c r="FX247"/>
     </row>
-    <row r="248" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A248" s="12" t="s">
         <v>38</v>
       </c>
@@ -43263,11 +43692,17 @@
         <v>6.2001471391325111</v>
       </c>
       <c r="FS248" s="11">
-        <v>6.9186294517084406</v>
-      </c>
+        <v>6.9511783319792215</v>
+      </c>
+      <c r="FT248" s="11">
+        <v>5.4736266240646785</v>
+      </c>
+      <c r="FU248"/>
       <c r="FV248"/>
+      <c r="FW248"/>
+      <c r="FX248"/>
     </row>
-    <row r="249" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A249" s="14"/>
       <c r="B249" s="11"/>
       <c r="C249" s="11"/>
@@ -43443,9 +43878,13 @@
       <c r="FQ249" s="11"/>
       <c r="FR249" s="11"/>
       <c r="FS249" s="11"/>
+      <c r="FT249" s="11"/>
+      <c r="FU249"/>
       <c r="FV249"/>
+      <c r="FW249"/>
+      <c r="FX249"/>
     </row>
-    <row r="250" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>10</v>
       </c>
@@ -43969,11 +44408,17 @@
         <v>5.3793620546446448</v>
       </c>
       <c r="FS250" s="11">
-        <v>5.4759513968919435</v>
-      </c>
+        <v>5.4874450057838402</v>
+      </c>
+      <c r="FT250" s="11">
+        <v>4.0025977978986447</v>
+      </c>
+      <c r="FU250"/>
       <c r="FV250"/>
+      <c r="FW250"/>
+      <c r="FX250"/>
     </row>
-    <row r="251" spans="1:178" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B251" s="16"/>
       <c r="C251" s="16"/>
       <c r="D251" s="16"/>
@@ -44148,9 +44593,12 @@
       <c r="FO251" s="16"/>
       <c r="FR251" s="16"/>
       <c r="FS251" s="16"/>
+      <c r="FU251"/>
       <c r="FV251"/>
+      <c r="FW251"/>
+      <c r="FX251"/>
     </row>
-    <row r="252" spans="1:178" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B252" s="16"/>
       <c r="C252" s="16"/>
       <c r="D252" s="16"/>
@@ -44321,9 +44769,12 @@
       <c r="FO252" s="16"/>
       <c r="FR252" s="16"/>
       <c r="FS252" s="16"/>
+      <c r="FU252"/>
       <c r="FV252"/>
+      <c r="FW252"/>
+      <c r="FX252"/>
     </row>
-    <row r="253" spans="1:178" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B253" s="16"/>
       <c r="C253" s="16"/>
       <c r="D253" s="16"/>
@@ -44501,15 +44952,21 @@
       </c>
       <c r="FO253" s="16"/>
       <c r="FR253" s="16">
-        <v>13.6558695901769</v>
+        <v>14.6558695901769</v>
       </c>
       <c r="FS253" s="16"/>
+      <c r="FU253"/>
       <c r="FV253"/>
+      <c r="FW253"/>
+      <c r="FX253"/>
     </row>
-    <row r="254" spans="1:178" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="FU254"/>
       <c r="FV254"/>
+      <c r="FW254"/>
+      <c r="FX254"/>
     </row>
-    <row r="255" spans="1:178" ht="7.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:180" ht="7.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="8"/>
       <c r="B255" s="8"/>
       <c r="C255" s="8"/>
@@ -44681,9 +45138,12 @@
       <c r="FO255" s="8"/>
       <c r="FR255" s="8"/>
       <c r="FS255" s="8"/>
+      <c r="FU255"/>
       <c r="FV255"/>
+      <c r="FW255"/>
+      <c r="FX255"/>
     </row>
-    <row r="256" spans="1:178" ht="15" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>0</v>
       </c>
@@ -44691,48 +45151,64 @@
       <c r="FM256" s="4"/>
       <c r="FP256" s="4"/>
       <c r="FQ256" s="4"/>
+      <c r="FT256" s="4"/>
+      <c r="FU256"/>
       <c r="FV256"/>
+      <c r="FW256"/>
+      <c r="FX256"/>
     </row>
-    <row r="257" spans="1:179" ht="15" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:180" ht="15" x14ac:dyDescent="0.25">
+      <c r="FU257"/>
       <c r="FV257"/>
+      <c r="FW257"/>
+      <c r="FX257"/>
     </row>
-    <row r="258" spans="1:179" ht="15" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:180" ht="15" x14ac:dyDescent="0.25">
+      <c r="FU258"/>
       <c r="FV258"/>
+      <c r="FW258"/>
+      <c r="FX258"/>
     </row>
-    <row r="259" spans="1:179" ht="15" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>8</v>
       </c>
       <c r="FU259"/>
+      <c r="FV259"/>
+      <c r="FW259"/>
+      <c r="FX259"/>
     </row>
-    <row r="260" spans="1:179" ht="15" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>7</v>
       </c>
       <c r="FU260"/>
+      <c r="FV260"/>
+      <c r="FW260"/>
+      <c r="FX260"/>
     </row>
-    <row r="261" spans="1:179" ht="15" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:180" ht="15" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>41</v>
       </c>
       <c r="FU261"/>
     </row>
-    <row r="263" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="264" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A264" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="265" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A265" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="267" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A267" s="4"/>
       <c r="B267" s="5">
         <v>1981</v>
@@ -45002,8 +45478,9 @@
         <v>2024</v>
       </c>
       <c r="FW267" s="5"/>
+      <c r="FX267" s="5"/>
     </row>
-    <row r="268" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A268" s="2" t="s">
         <v>13</v>
       </c>
@@ -45541,8 +46018,11 @@
       <c r="FW268" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="FX268" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="270" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A270" s="12" t="s">
         <v>36</v>
       </c>
@@ -46078,10 +46558,13 @@
         <v>9.5228757968063924</v>
       </c>
       <c r="FW270" s="11">
-        <v>8.0959782197010313</v>
+        <v>8.0914546523495279</v>
+      </c>
+      <c r="FX270" s="11">
+        <v>8.0301164949525425</v>
       </c>
     </row>
-    <row r="271" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A271" s="12" t="s">
         <v>37</v>
       </c>
@@ -46617,10 +47100,13 @@
         <v>28.179113259676331</v>
       </c>
       <c r="FW271" s="11">
-        <v>28.44551377144392</v>
+        <v>28.446122155938291</v>
+      </c>
+      <c r="FX271" s="11">
+        <v>23.62085785765845</v>
       </c>
     </row>
-    <row r="272" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A272" s="12" t="s">
         <v>38</v>
       </c>
@@ -47156,10 +47642,13 @@
         <v>62.298010943517269</v>
       </c>
       <c r="FW272" s="11">
-        <v>63.458508008855055</v>
+        <v>63.462423191712183</v>
+      </c>
+      <c r="FX272" s="11">
+        <v>68.349025647388999</v>
       </c>
     </row>
-    <row r="273" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A273" s="14"/>
       <c r="B273" s="11"/>
       <c r="C273" s="11"/>
@@ -47339,8 +47828,9 @@
       <c r="FU273" s="11"/>
       <c r="FV273" s="11"/>
       <c r="FW273" s="11"/>
+      <c r="FX273" s="11"/>
     </row>
-    <row r="274" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A274" s="7" t="s">
         <v>10</v>
       </c>
@@ -47878,8 +48368,11 @@
       <c r="FW274" s="11">
         <v>100</v>
       </c>
+      <c r="FX274" s="11">
+        <v>100</v>
+      </c>
     </row>
-    <row r="275" spans="1:179" s="13" customFormat="1" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:180" s="13" customFormat="1" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A275" s="1"/>
       <c r="FB275" s="13">
         <v>20558.222744577564</v>
@@ -47888,10 +48381,10 @@
         <v>-24370.119758612476</v>
       </c>
     </row>
-    <row r="276" spans="1:179" s="13" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:180" s="13" customFormat="1" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A276" s="1"/>
     </row>
-    <row r="277" spans="1:179" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="FB277" s="1">
         <v>4422950.8840171499</v>
       </c>
@@ -47899,8 +48392,8 @@
         <v>4857262.3839106075</v>
       </c>
     </row>
-    <row r="278" spans="1:179" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="279" spans="1:179" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:180" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="279" spans="1:180" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A279" s="8"/>
       <c r="B279" s="8"/>
       <c r="C279" s="8"/>
@@ -48080,49 +48573,50 @@
       <c r="FU279" s="8"/>
       <c r="FV279" s="8"/>
       <c r="FW279" s="8"/>
+      <c r="FX279" s="8"/>
     </row>
-    <row r="280" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A280" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A283" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="284" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A284" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="285" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A285" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="287" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A287" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="288" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A288" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="289" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A289" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="290" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:180" x14ac:dyDescent="0.2">
       <c r="FJ290" s="8"/>
       <c r="FN290" s="8"/>
       <c r="FR290" s="8"/>
       <c r="FV290" s="8"/>
     </row>
-    <row r="291" spans="1:179" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:180" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A291" s="4"/>
       <c r="B291" s="5">
         <v>1981</v>
@@ -48392,8 +48886,9 @@
         <v>2025</v>
       </c>
       <c r="FW291" s="5"/>
+      <c r="FX291" s="5"/>
     </row>
-    <row r="292" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A292" s="2" t="s">
         <v>13</v>
       </c>
@@ -48931,8 +49426,11 @@
       <c r="FW292" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="FX292" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="294" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A294" s="12" t="s">
         <v>36</v>
       </c>
@@ -49468,10 +49966,13 @@
         <v>8.3447197209876212</v>
       </c>
       <c r="FW294" s="11">
-        <v>7.4701295913301378</v>
+        <v>7.469465493208534</v>
+      </c>
+      <c r="FX294" s="11">
+        <v>7.4312999321726814</v>
       </c>
     </row>
-    <row r="295" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A295" s="12" t="s">
         <v>37</v>
       </c>
@@ -50007,10 +50508,13 @@
         <v>29.534417043326695</v>
       </c>
       <c r="FW295" s="11">
-        <v>29.293470233458478</v>
+        <v>29.281775640038362</v>
+      </c>
+      <c r="FX295" s="11">
+        <v>25.871921555991346</v>
       </c>
     </row>
-    <row r="296" spans="1:179" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:180" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A296" s="12" t="s">
         <v>38</v>
       </c>
@@ -50546,10 +51050,13 @@
         <v>62.12086323568569</v>
       </c>
       <c r="FW296" s="11">
-        <v>63.236400175211372</v>
+        <v>63.248758866753121</v>
+      </c>
+      <c r="FX296" s="11">
+        <v>66.696778511835959</v>
       </c>
     </row>
-    <row r="297" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A297" s="14"/>
       <c r="B297" s="11"/>
       <c r="C297" s="11"/>
@@ -50729,8 +51236,9 @@
       <c r="FU297" s="11"/>
       <c r="FV297" s="11"/>
       <c r="FW297" s="11"/>
+      <c r="FX297" s="11"/>
     </row>
-    <row r="298" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A298" s="7" t="s">
         <v>10</v>
       </c>
@@ -51268,8 +51776,11 @@
       <c r="FW298" s="11">
         <v>100</v>
       </c>
+      <c r="FX298" s="11">
+        <v>100</v>
+      </c>
     </row>
-    <row r="299" spans="1:179" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:180" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="FB299" s="1" t="e">
         <v>#DIV/0!</v>
       </c>
@@ -51277,7 +51788,7 @@
         <v>-0.58654919688841323</v>
       </c>
     </row>
-    <row r="300" spans="1:179" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:180" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="FB300" s="1" t="e">
         <v>#DIV/0!</v>
       </c>
@@ -51285,7 +51796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:179" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:180" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="FB301" s="1" t="e">
         <v>#DIV/0!</v>
       </c>
@@ -51293,7 +51804,7 @@
         <v>116.90641566717015</v>
       </c>
     </row>
-    <row r="302" spans="1:179" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:180" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="FB302" s="1" t="e">
         <v>#DIV/0!</v>
       </c>
@@ -51301,7 +51812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:179" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:180" ht="7.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A303" s="8"/>
       <c r="B303" s="8"/>
       <c r="C303" s="8"/>
@@ -51481,70 +51992,71 @@
       <c r="FU303" s="8"/>
       <c r="FV303" s="8"/>
       <c r="FW303" s="8"/>
+      <c r="FX303" s="8"/>
     </row>
-    <row r="304" spans="1:179" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:180" x14ac:dyDescent="0.2">
       <c r="A304" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="B147:BY147 CA147:FW147">
+  <conditionalFormatting sqref="B147:BY147 CA147:FX147">
     <cfRule type="cellIs" dxfId="11" priority="11" operator="greaterThanOrEqual">
       <formula>1000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B294:BY294 CA294:FW294">
+  <conditionalFormatting sqref="B294:BY294 CA294:FX294">
     <cfRule type="cellIs" dxfId="10" priority="7" operator="greaterThanOrEqual">
       <formula>1000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B66:FS73">
+  <conditionalFormatting sqref="B66:FT73">
     <cfRule type="cellIs" dxfId="9" priority="14" operator="greaterThanOrEqual">
       <formula>1000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B93:FS100">
+  <conditionalFormatting sqref="B93:FT100">
     <cfRule type="cellIs" dxfId="8" priority="6" operator="greaterThanOrEqual">
       <formula>1000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B222:FS226">
+  <conditionalFormatting sqref="B222:FT226">
     <cfRule type="cellIs" dxfId="7" priority="10" operator="greaterThanOrEqual">
       <formula>1000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B246:FS250">
+  <conditionalFormatting sqref="B246:FT250">
     <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThanOrEqual">
       <formula>1000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B120:FW127">
+  <conditionalFormatting sqref="B120:FX127">
     <cfRule type="cellIs" dxfId="5" priority="12" operator="greaterThanOrEqual">
       <formula>1000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B148:FW154">
+  <conditionalFormatting sqref="B148:FX154">
     <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThanOrEqual">
       <formula>1000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B270:FW274">
+  <conditionalFormatting sqref="B270:FX274">
     <cfRule type="cellIs" dxfId="3" priority="8" operator="greaterThanOrEqual">
       <formula>1000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B295:FW298">
+  <conditionalFormatting sqref="B295:FX298">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThanOrEqual">
       <formula>1000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BZ147:FW151">
+  <conditionalFormatting sqref="BZ147:FX151">
     <cfRule type="cellIs" dxfId="1" priority="5" operator="greaterThanOrEqual">
       <formula>1000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BZ294:FW296">
+  <conditionalFormatting sqref="BZ294:FX296">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThanOrEqual">
       <formula>1000</formula>
     </cfRule>

</xml_diff>